<commit_message>
new - cash in record
</commit_message>
<xml_diff>
--- a/investment/record.xlsx
+++ b/investment/record.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="11640"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="11640" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="损益" sheetId="1" r:id="rId1"/>
@@ -184,7 +184,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -237,9 +237,6 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="7" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -550,7 +547,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
@@ -590,7 +587,7 @@
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="20" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="4">
@@ -610,7 +607,7 @@
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="21"/>
+      <c r="A3" s="20"/>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
@@ -619,7 +616,7 @@
       <c r="G3" s="8"/>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="21"/>
+      <c r="A4" s="20"/>
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
@@ -628,7 +625,7 @@
       <c r="G4" s="8"/>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="21"/>
+      <c r="A5" s="20"/>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
@@ -637,7 +634,7 @@
       <c r="G5" s="8"/>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="20" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="4">
@@ -657,7 +654,7 @@
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="21"/>
+      <c r="A7" s="20"/>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
@@ -666,7 +663,7 @@
       <c r="G7" s="11"/>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="21"/>
+      <c r="A8" s="20"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
@@ -675,7 +672,7 @@
       <c r="G8" s="11"/>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="21"/>
+      <c r="A9" s="20"/>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
@@ -684,7 +681,7 @@
       <c r="G9" s="11"/>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="21" t="s">
+      <c r="A10" s="20" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="4">
@@ -706,7 +703,7 @@
       </c>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="21"/>
+      <c r="A11" s="20"/>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
@@ -715,7 +712,7 @@
       <c r="G11" s="7"/>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="21"/>
+      <c r="A12" s="20"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
@@ -724,7 +721,7 @@
       <c r="G12" s="7"/>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="21"/>
+      <c r="A13" s="20"/>
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
@@ -748,8 +745,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
@@ -783,7 +780,7 @@
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="21" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="16">
@@ -804,7 +801,7 @@
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="22"/>
+      <c r="A3" s="21"/>
       <c r="B3" s="16">
         <v>42045</v>
       </c>
@@ -823,7 +820,7 @@
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="22"/>
+      <c r="A4" s="21"/>
       <c r="B4" s="16">
         <v>42051</v>
       </c>
@@ -842,7 +839,7 @@
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="22"/>
+      <c r="A5" s="21"/>
       <c r="B5" s="16">
         <v>42063</v>
       </c>
@@ -861,99 +858,134 @@
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="22"/>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
+      <c r="A6" s="21"/>
+      <c r="B6" s="16">
+        <v>42068</v>
+      </c>
+      <c r="C6" s="17">
+        <v>7000</v>
+      </c>
+      <c r="D6" s="17">
+        <v>0</v>
+      </c>
+      <c r="E6" s="17">
+        <v>0</v>
+      </c>
+      <c r="F6" s="17">
+        <f>F5+C6-D6+E6</f>
+        <v>198462.69999999998</v>
+      </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="22"/>
-      <c r="B7" s="19"/>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="19"/>
-      <c r="F7" s="19"/>
+      <c r="A7" s="21"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="17">
+        <v>0</v>
+      </c>
+      <c r="D7" s="17">
+        <v>0</v>
+      </c>
+      <c r="E7" s="17">
+        <v>0</v>
+      </c>
+      <c r="F7" s="18"/>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="22"/>
-      <c r="B8" s="19"/>
-      <c r="C8" s="19"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="19"/>
-      <c r="F8" s="19"/>
+      <c r="A8" s="21"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="17">
+        <v>0</v>
+      </c>
+      <c r="D8" s="17">
+        <v>0</v>
+      </c>
+      <c r="E8" s="17">
+        <v>0</v>
+      </c>
+      <c r="F8" s="18"/>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="22"/>
-      <c r="B9" s="19"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="19"/>
+      <c r="A9" s="21"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="17">
+        <v>0</v>
+      </c>
+      <c r="D9" s="17">
+        <v>0</v>
+      </c>
+      <c r="E9" s="17">
+        <v>0</v>
+      </c>
+      <c r="F9" s="18"/>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="22"/>
-      <c r="B10" s="19"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="19"/>
+      <c r="A10" s="21"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="17">
+        <v>0</v>
+      </c>
+      <c r="D10" s="17">
+        <v>0</v>
+      </c>
+      <c r="E10" s="17">
+        <v>0</v>
+      </c>
+      <c r="F10" s="18"/>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="22" t="s">
+      <c r="A11" s="21" t="s">
         <v>14</v>
       </c>
       <c r="B11" s="16">
         <v>41639</v>
       </c>
-      <c r="C11" s="20">
+      <c r="C11" s="19">
         <v>13684</v>
       </c>
-      <c r="D11" s="20">
-        <v>0</v>
-      </c>
-      <c r="E11" s="20">
-        <v>0</v>
-      </c>
-      <c r="F11" s="20">
+      <c r="D11" s="19">
+        <v>0</v>
+      </c>
+      <c r="E11" s="19">
+        <v>0</v>
+      </c>
+      <c r="F11" s="19">
         <v>13684</v>
       </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="22"/>
+      <c r="A12" s="21"/>
       <c r="B12" s="16">
         <v>41992</v>
       </c>
-      <c r="C12" s="20">
+      <c r="C12" s="19">
         <v>3071.25</v>
       </c>
-      <c r="D12" s="20">
-        <v>0</v>
-      </c>
-      <c r="E12" s="20">
-        <v>0</v>
-      </c>
-      <c r="F12" s="20">
+      <c r="D12" s="19">
+        <v>0</v>
+      </c>
+      <c r="E12" s="19">
+        <v>0</v>
+      </c>
+      <c r="F12" s="19">
         <f>F11+C12-D12+E12</f>
         <v>16755.25</v>
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="22"/>
+      <c r="A13" s="21"/>
       <c r="B13" s="16">
         <v>42004</v>
       </c>
-      <c r="C13" s="20">
+      <c r="C13" s="19">
         <v>14393.08</v>
       </c>
-      <c r="D13" s="20">
-        <v>0</v>
-      </c>
-      <c r="E13" s="20">
-        <v>0</v>
-      </c>
-      <c r="F13" s="20">
+      <c r="D13" s="19">
+        <v>0</v>
+      </c>
+      <c r="E13" s="19">
+        <v>0</v>
+      </c>
+      <c r="F13" s="19">
         <f>F12+C13-D13+E13</f>
         <v>31148.33</v>
       </c>

</xml_diff>

<commit_message>
new - transaction record
</commit_message>
<xml_diff>
--- a/investment/record.xlsx
+++ b/investment/record.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="11640" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="11640" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="损益" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="40">
   <si>
     <t>日期</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -79,6 +79,102 @@
   </si>
   <si>
     <t>资产收益率（ROE）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>代码</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>名称</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>日期</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>价格</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>数量</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SH-601168</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>西部矿业</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>类型</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>B</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>收益率</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>日收益率</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SZ-000671</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>阳光城</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>S</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SZ-000629</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>攀钢钒钛</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>S</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SZ-300217</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>东方电热</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>S</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>中国建筑</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SH-610668</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SZ-000777</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>中核科技</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -92,7 +188,7 @@
     <numFmt numFmtId="177" formatCode="&quot;US$&quot;#,##0.00;\-&quot;US$&quot;#,##0.00"/>
     <numFmt numFmtId="178" formatCode="&quot;¥&quot;#,##0.00_);[Red]\(&quot;¥&quot;#,##0.00\)"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -140,6 +236,22 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF00B050"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -184,7 +296,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -240,16 +352,49 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -587,7 +732,7 @@
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="22" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="4">
@@ -607,7 +752,7 @@
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="20"/>
+      <c r="A3" s="22"/>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
@@ -616,7 +761,7 @@
       <c r="G3" s="8"/>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="20"/>
+      <c r="A4" s="22"/>
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
@@ -625,7 +770,7 @@
       <c r="G4" s="8"/>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="20"/>
+      <c r="A5" s="22"/>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
@@ -634,7 +779,7 @@
       <c r="G5" s="8"/>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="22" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="4">
@@ -654,7 +799,7 @@
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="20"/>
+      <c r="A7" s="22"/>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
@@ -663,7 +808,7 @@
       <c r="G7" s="11"/>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="20"/>
+      <c r="A8" s="22"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
@@ -672,7 +817,7 @@
       <c r="G8" s="11"/>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="20"/>
+      <c r="A9" s="22"/>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
@@ -681,7 +826,7 @@
       <c r="G9" s="11"/>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="20" t="s">
+      <c r="A10" s="22" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="4">
@@ -703,7 +848,7 @@
       </c>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="20"/>
+      <c r="A11" s="22"/>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
@@ -712,7 +857,7 @@
       <c r="G11" s="7"/>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="20"/>
+      <c r="A12" s="22"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
@@ -721,7 +866,7 @@
       <c r="G12" s="7"/>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="20"/>
+      <c r="A13" s="22"/>
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
@@ -745,7 +890,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
@@ -780,7 +925,7 @@
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="23" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="16">
@@ -801,7 +946,7 @@
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="21"/>
+      <c r="A3" s="23"/>
       <c r="B3" s="16">
         <v>42045</v>
       </c>
@@ -820,7 +965,7 @@
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="21"/>
+      <c r="A4" s="23"/>
       <c r="B4" s="16">
         <v>42051</v>
       </c>
@@ -839,7 +984,7 @@
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="21"/>
+      <c r="A5" s="23"/>
       <c r="B5" s="16">
         <v>42063</v>
       </c>
@@ -858,7 +1003,7 @@
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="21"/>
+      <c r="A6" s="23"/>
       <c r="B6" s="16">
         <v>42068</v>
       </c>
@@ -877,8 +1022,8 @@
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="21"/>
-      <c r="B7" s="18"/>
+      <c r="A7" s="23"/>
+      <c r="B7" s="19"/>
       <c r="C7" s="17">
         <v>0</v>
       </c>
@@ -888,11 +1033,11 @@
       <c r="E7" s="17">
         <v>0</v>
       </c>
-      <c r="F7" s="18"/>
+      <c r="F7" s="19"/>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="21"/>
-      <c r="B8" s="18"/>
+      <c r="A8" s="23"/>
+      <c r="B8" s="19"/>
       <c r="C8" s="17">
         <v>0</v>
       </c>
@@ -902,11 +1047,11 @@
       <c r="E8" s="17">
         <v>0</v>
       </c>
-      <c r="F8" s="18"/>
+      <c r="F8" s="19"/>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="21"/>
-      <c r="B9" s="18"/>
+      <c r="A9" s="23"/>
+      <c r="B9" s="19"/>
       <c r="C9" s="17">
         <v>0</v>
       </c>
@@ -916,11 +1061,11 @@
       <c r="E9" s="17">
         <v>0</v>
       </c>
-      <c r="F9" s="18"/>
+      <c r="F9" s="19"/>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="21"/>
-      <c r="B10" s="18"/>
+      <c r="A10" s="23"/>
+      <c r="B10" s="19"/>
       <c r="C10" s="17">
         <v>0</v>
       </c>
@@ -930,62 +1075,62 @@
       <c r="E10" s="17">
         <v>0</v>
       </c>
-      <c r="F10" s="18"/>
+      <c r="F10" s="19"/>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="21" t="s">
+      <c r="A11" s="23" t="s">
         <v>14</v>
       </c>
       <c r="B11" s="16">
         <v>41639</v>
       </c>
-      <c r="C11" s="19">
+      <c r="C11" s="20">
         <v>13684</v>
       </c>
-      <c r="D11" s="19">
-        <v>0</v>
-      </c>
-      <c r="E11" s="19">
-        <v>0</v>
-      </c>
-      <c r="F11" s="19">
+      <c r="D11" s="20">
+        <v>0</v>
+      </c>
+      <c r="E11" s="20">
+        <v>0</v>
+      </c>
+      <c r="F11" s="20">
         <v>13684</v>
       </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="21"/>
+      <c r="A12" s="23"/>
       <c r="B12" s="16">
         <v>41992</v>
       </c>
-      <c r="C12" s="19">
+      <c r="C12" s="20">
         <v>3071.25</v>
       </c>
-      <c r="D12" s="19">
-        <v>0</v>
-      </c>
-      <c r="E12" s="19">
-        <v>0</v>
-      </c>
-      <c r="F12" s="19">
+      <c r="D12" s="20">
+        <v>0</v>
+      </c>
+      <c r="E12" s="20">
+        <v>0</v>
+      </c>
+      <c r="F12" s="20">
         <f>F11+C12-D12+E12</f>
         <v>16755.25</v>
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="21"/>
+      <c r="A13" s="23"/>
       <c r="B13" s="16">
         <v>42004</v>
       </c>
-      <c r="C13" s="19">
+      <c r="C13" s="20">
         <v>14393.08</v>
       </c>
-      <c r="D13" s="19">
-        <v>0</v>
-      </c>
-      <c r="E13" s="19">
-        <v>0</v>
-      </c>
-      <c r="F13" s="19">
+      <c r="D13" s="20">
+        <v>0</v>
+      </c>
+      <c r="E13" s="20">
+        <v>0</v>
+      </c>
+      <c r="F13" s="20">
         <f>F12+C13-D13+E13</f>
         <v>31148.33</v>
       </c>
@@ -1073,15 +1218,459 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="12"/>
+  <cols>
+    <col min="1" max="1" width="11.625" style="14" customWidth="1"/>
+    <col min="2" max="2" width="9" style="14"/>
+    <col min="3" max="3" width="10.25" style="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="9" style="14"/>
+    <col min="8" max="8" width="9.625" style="14" customWidth="1"/>
+    <col min="9" max="16384" width="9" style="14"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="15" customHeight="1">
+      <c r="A1" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" s="21" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="16">
+        <v>41981</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="18">
+        <v>9.9</v>
+      </c>
+      <c r="F2" s="18">
+        <v>1000</v>
+      </c>
+      <c r="G2" s="18"/>
+      <c r="H2" s="25"/>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="18"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="26">
+        <v>41985</v>
+      </c>
+      <c r="D3" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" s="30">
+        <v>10.37</v>
+      </c>
+      <c r="F3" s="30">
+        <v>1000</v>
+      </c>
+      <c r="G3" s="11">
+        <v>4.5400000000000003E-2</v>
+      </c>
+      <c r="H3" s="11">
+        <f>G3/5</f>
+        <v>9.0800000000000013E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="16">
+        <v>42003</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="18">
+        <v>7.11</v>
+      </c>
+      <c r="F4" s="18">
+        <v>1600</v>
+      </c>
+      <c r="G4" s="18"/>
+      <c r="H4" s="25"/>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="18"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="26">
+        <v>42011</v>
+      </c>
+      <c r="D5" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="30">
+        <v>7.14</v>
+      </c>
+      <c r="F5" s="30">
+        <v>1600</v>
+      </c>
+      <c r="G5" s="11">
+        <v>2.2000000000000001E-3</v>
+      </c>
+      <c r="H5" s="11">
+        <f>G5/9</f>
+        <v>2.4444444444444448E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="16">
+        <v>41992</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="18">
+        <v>12.52</v>
+      </c>
+      <c r="F6" s="18">
+        <v>800</v>
+      </c>
+      <c r="G6" s="18"/>
+      <c r="H6" s="25"/>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="18"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="26">
+        <v>42003</v>
+      </c>
+      <c r="D7" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="27">
+        <v>13.9</v>
+      </c>
+      <c r="F7" s="27">
+        <v>800</v>
+      </c>
+      <c r="G7" s="11">
+        <v>0.108</v>
+      </c>
+      <c r="H7" s="11">
+        <f>G7/12</f>
+        <v>8.9999999999999993E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="16">
+        <v>41985</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="18">
+        <v>3.47</v>
+      </c>
+      <c r="F8" s="18">
+        <v>3000</v>
+      </c>
+      <c r="G8" s="18"/>
+      <c r="H8" s="25"/>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="18"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="28">
+        <v>41992</v>
+      </c>
+      <c r="D9" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="29">
+        <v>3.47</v>
+      </c>
+      <c r="F9" s="29">
+        <v>3000</v>
+      </c>
+      <c r="G9" s="8">
+        <v>-2E-3</v>
+      </c>
+      <c r="H9" s="8">
+        <f>G9/8</f>
+        <v>-2.5000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="16">
+        <v>40695</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="18">
+        <v>16.34</v>
+      </c>
+      <c r="F10" s="18">
+        <v>1080</v>
+      </c>
+      <c r="G10" s="8"/>
+      <c r="H10" s="25"/>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="18"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="26">
+        <v>41954</v>
+      </c>
+      <c r="D11" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="30">
+        <v>27.55</v>
+      </c>
+      <c r="F11" s="30">
+        <v>780</v>
+      </c>
+      <c r="G11" s="11"/>
+      <c r="H11" s="32"/>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="18"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="31">
+        <v>41970</v>
+      </c>
+      <c r="D12" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" s="30">
+        <v>30.2</v>
+      </c>
+      <c r="F12" s="30">
+        <v>300</v>
+      </c>
+      <c r="G12" s="11">
+        <v>0.72070000000000001</v>
+      </c>
+      <c r="H12" s="32">
+        <f>G12/1273</f>
+        <v>5.6614296936370774E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="16">
+        <v>42011</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" s="18">
+        <v>10.11</v>
+      </c>
+      <c r="F13" s="18">
+        <v>1100</v>
+      </c>
+      <c r="G13" s="18"/>
+      <c r="H13" s="25"/>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="18"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="25"/>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="18"/>
+      <c r="B15" s="18"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="25"/>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="18"/>
+      <c r="B16" s="18"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="25"/>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="18"/>
+      <c r="B17" s="18"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="25"/>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="18"/>
+      <c r="B18" s="18"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
+      <c r="H18" s="25"/>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="18"/>
+      <c r="B19" s="18"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="25"/>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="18"/>
+      <c r="B20" s="18"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
+      <c r="H20" s="25"/>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="18"/>
+      <c r="B21" s="18"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="25"/>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="18"/>
+      <c r="B22" s="18"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="25"/>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="18"/>
+      <c r="B23" s="18"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="25"/>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" s="18"/>
+      <c r="B24" s="18"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
+      <c r="H24" s="25"/>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="H25" s="24"/>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="H26" s="24"/>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="H27" s="24"/>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="H28" s="24"/>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="H29" s="24"/>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="H30" s="24"/>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="H31" s="24"/>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="H32" s="24"/>
+    </row>
+    <row r="33" spans="8:8">
+      <c r="H33" s="24"/>
+    </row>
+    <row r="34" spans="8:8">
+      <c r="H34" s="24"/>
+    </row>
+    <row r="35" spans="8:8">
+      <c r="H35" s="24"/>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
new - cash source
</commit_message>
<xml_diff>
--- a/investment/record.xlsx
+++ b/investment/record.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="11640" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="8220" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="损益" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="43">
   <si>
     <t>日期</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -175,6 +175,18 @@
   </si>
   <si>
     <t>中核科技</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>资金来源</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>老婆2月工资</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>我2014年终奖</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -296,7 +308,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -304,9 +316,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -709,170 +718,170 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" ht="18" customHeight="1">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="15" t="s">
+      <c r="B1" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="G1" s="14" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="3">
         <v>42005</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="4">
         <v>160000</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D2" s="5">
         <v>156424.13</v>
       </c>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="8">
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="7">
         <f>(D2-C2)/C2</f>
         <v>-2.2349187499999972E-2</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="22"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="8"/>
+      <c r="A3" s="21"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="7"/>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="22"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="8"/>
+      <c r="A4" s="21"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="7"/>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="22"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="8"/>
+      <c r="A5" s="21"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="7"/>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="3">
         <v>42005</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="8">
         <v>31148.33</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="9">
         <v>31678.66</v>
       </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="11">
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="10">
         <f t="shared" ref="G6:G10" si="0">(D6-C6)/C6</f>
         <v>1.7025952916255801E-2</v>
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="22"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="11"/>
+      <c r="A7" s="21"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="10"/>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="22"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="11"/>
+      <c r="A8" s="21"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="10"/>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="22"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="11"/>
+      <c r="A9" s="21"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="10"/>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="22" t="s">
+      <c r="A10" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="3">
         <v>42005</v>
       </c>
-      <c r="C10" s="12">
+      <c r="C10" s="11">
         <f>C6*6.2743+C2</f>
         <v>355433.96691900003</v>
       </c>
-      <c r="D10" s="13">
+      <c r="D10" s="12">
         <f>D6*6.2743+D2</f>
         <v>355185.54643800005</v>
       </c>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="8">
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="7">
         <f t="shared" si="0"/>
         <v>-6.9892161166631495E-4</v>
       </c>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="22"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
+      <c r="A11" s="21"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="22"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
+      <c r="A12" s="21"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="22"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
+      <c r="A13" s="21"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -888,10 +897,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
@@ -901,309 +910,329 @@
     <col min="3" max="3" width="14.375" style="1" customWidth="1"/>
     <col min="4" max="5" width="13.625" style="1" customWidth="1"/>
     <col min="6" max="6" width="17.125" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="9" style="1"/>
+    <col min="7" max="7" width="12.375" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16.5" customHeight="1">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:7" ht="16.5" customHeight="1">
+      <c r="A1" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="B1" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="20" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="23" t="s">
+      <c r="G1" s="20" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="16">
+      <c r="B2" s="15">
         <v>42005</v>
       </c>
-      <c r="C2" s="17">
+      <c r="C2" s="16">
         <v>160000</v>
       </c>
-      <c r="D2" s="17">
-        <v>0</v>
-      </c>
-      <c r="E2" s="17">
-        <v>0</v>
-      </c>
-      <c r="F2" s="17">
+      <c r="D2" s="16">
+        <v>0</v>
+      </c>
+      <c r="E2" s="16">
+        <v>0</v>
+      </c>
+      <c r="F2" s="16">
         <f>C2-D2+E2</f>
         <v>160000</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="23"/>
-      <c r="B3" s="16">
+      <c r="G2" s="18"/>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="22"/>
+      <c r="B3" s="15">
         <v>42045</v>
       </c>
-      <c r="C3" s="17">
-        <v>0</v>
-      </c>
-      <c r="D3" s="17">
-        <v>0</v>
-      </c>
-      <c r="E3" s="17">
+      <c r="C3" s="16">
+        <v>0</v>
+      </c>
+      <c r="D3" s="16">
+        <v>0</v>
+      </c>
+      <c r="E3" s="16">
         <v>403.09</v>
       </c>
-      <c r="F3" s="17">
+      <c r="F3" s="16">
         <f>F2+C3-D3+E3</f>
         <v>160403.09</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="23"/>
-      <c r="B4" s="16">
+      <c r="G3" s="18"/>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="22"/>
+      <c r="B4" s="15">
         <v>42051</v>
       </c>
-      <c r="C4" s="17">
+      <c r="C4" s="16">
         <v>31000</v>
       </c>
-      <c r="D4" s="17">
-        <v>0</v>
-      </c>
-      <c r="E4" s="17">
-        <v>0</v>
-      </c>
-      <c r="F4" s="17">
+      <c r="D4" s="16">
+        <v>0</v>
+      </c>
+      <c r="E4" s="16">
+        <v>0</v>
+      </c>
+      <c r="F4" s="16">
         <f>F3+C4-D4+E4</f>
         <v>191403.09</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="23"/>
-      <c r="B5" s="16">
+      <c r="G4" s="18" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="22"/>
+      <c r="B5" s="15">
         <v>42063</v>
       </c>
-      <c r="C5" s="17">
-        <v>0</v>
-      </c>
-      <c r="D5" s="17">
-        <v>0</v>
-      </c>
-      <c r="E5" s="17">
+      <c r="C5" s="16">
+        <v>0</v>
+      </c>
+      <c r="D5" s="16">
+        <v>0</v>
+      </c>
+      <c r="E5" s="16">
         <v>59.61</v>
       </c>
-      <c r="F5" s="17">
+      <c r="F5" s="16">
         <f>F4+C5-D5+E5</f>
         <v>191462.69999999998</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="23"/>
-      <c r="B6" s="16">
+      <c r="G5" s="18"/>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="22"/>
+      <c r="B6" s="15">
         <v>42068</v>
       </c>
-      <c r="C6" s="17">
+      <c r="C6" s="16">
         <v>7000</v>
       </c>
-      <c r="D6" s="17">
-        <v>0</v>
-      </c>
-      <c r="E6" s="17">
-        <v>0</v>
-      </c>
-      <c r="F6" s="17">
+      <c r="D6" s="16">
+        <v>0</v>
+      </c>
+      <c r="E6" s="16">
+        <v>0</v>
+      </c>
+      <c r="F6" s="16">
         <f>F5+C6-D6+E6</f>
         <v>198462.69999999998</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="23"/>
-      <c r="B7" s="19"/>
-      <c r="C7" s="17">
-        <v>0</v>
-      </c>
-      <c r="D7" s="17">
-        <v>0</v>
-      </c>
-      <c r="E7" s="17">
-        <v>0</v>
-      </c>
-      <c r="F7" s="19"/>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="23"/>
-      <c r="B8" s="19"/>
-      <c r="C8" s="17">
-        <v>0</v>
-      </c>
-      <c r="D8" s="17">
-        <v>0</v>
-      </c>
-      <c r="E8" s="17">
-        <v>0</v>
-      </c>
-      <c r="F8" s="19"/>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="23"/>
-      <c r="B9" s="19"/>
-      <c r="C9" s="17">
-        <v>0</v>
-      </c>
-      <c r="D9" s="17">
-        <v>0</v>
-      </c>
-      <c r="E9" s="17">
-        <v>0</v>
-      </c>
-      <c r="F9" s="19"/>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="23"/>
-      <c r="B10" s="19"/>
-      <c r="C10" s="17">
-        <v>0</v>
-      </c>
-      <c r="D10" s="17">
-        <v>0</v>
-      </c>
-      <c r="E10" s="17">
-        <v>0</v>
-      </c>
-      <c r="F10" s="19"/>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="23" t="s">
+      <c r="G6" s="18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="22"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="16">
+        <v>0</v>
+      </c>
+      <c r="D7" s="16">
+        <v>0</v>
+      </c>
+      <c r="E7" s="16">
+        <v>0</v>
+      </c>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="22"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="16">
+        <v>0</v>
+      </c>
+      <c r="D8" s="16">
+        <v>0</v>
+      </c>
+      <c r="E8" s="16">
+        <v>0</v>
+      </c>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="22"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="16">
+        <v>0</v>
+      </c>
+      <c r="D9" s="16">
+        <v>0</v>
+      </c>
+      <c r="E9" s="16">
+        <v>0</v>
+      </c>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="22"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="16">
+        <v>0</v>
+      </c>
+      <c r="D10" s="16">
+        <v>0</v>
+      </c>
+      <c r="E10" s="16">
+        <v>0</v>
+      </c>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="16">
+      <c r="B11" s="15">
         <v>41639</v>
       </c>
-      <c r="C11" s="20">
+      <c r="C11" s="19">
         <v>13684</v>
       </c>
-      <c r="D11" s="20">
-        <v>0</v>
-      </c>
-      <c r="E11" s="20">
-        <v>0</v>
-      </c>
-      <c r="F11" s="20">
+      <c r="D11" s="19">
+        <v>0</v>
+      </c>
+      <c r="E11" s="19">
+        <v>0</v>
+      </c>
+      <c r="F11" s="19">
         <v>13684</v>
       </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="23"/>
-      <c r="B12" s="16">
+      <c r="G11" s="18"/>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="22"/>
+      <c r="B12" s="15">
         <v>41992</v>
       </c>
-      <c r="C12" s="20">
+      <c r="C12" s="19">
         <v>3071.25</v>
       </c>
-      <c r="D12" s="20">
-        <v>0</v>
-      </c>
-      <c r="E12" s="20">
-        <v>0</v>
-      </c>
-      <c r="F12" s="20">
+      <c r="D12" s="19">
+        <v>0</v>
+      </c>
+      <c r="E12" s="19">
+        <v>0</v>
+      </c>
+      <c r="F12" s="19">
         <f>F11+C12-D12+E12</f>
         <v>16755.25</v>
       </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="23"/>
-      <c r="B13" s="16">
+      <c r="G12" s="18"/>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="22"/>
+      <c r="B13" s="15">
         <v>42004</v>
       </c>
-      <c r="C13" s="20">
+      <c r="C13" s="19">
         <v>14393.08</v>
       </c>
-      <c r="D13" s="20">
-        <v>0</v>
-      </c>
-      <c r="E13" s="20">
-        <v>0</v>
-      </c>
-      <c r="F13" s="20">
+      <c r="D13" s="19">
+        <v>0</v>
+      </c>
+      <c r="E13" s="19">
+        <v>0</v>
+      </c>
+      <c r="F13" s="19">
         <f>F12+C13-D13+E13</f>
         <v>31148.33</v>
       </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="B14" s="14"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="B16" s="14"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
+      <c r="G13" s="18"/>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="B15" s="13"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="B16" s="13"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
     </row>
     <row r="17" spans="2:6">
-      <c r="B17" s="14"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
     </row>
     <row r="18" spans="2:6">
-      <c r="B18" s="14"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
     </row>
     <row r="19" spans="2:6">
-      <c r="B19" s="14"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
     </row>
     <row r="20" spans="2:6">
-      <c r="B20" s="14"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
     </row>
     <row r="21" spans="2:6">
-      <c r="B21" s="14"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
     </row>
     <row r="22" spans="2:6">
-      <c r="B22" s="14"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
+      <c r="B22" s="13"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
     </row>
     <row r="23" spans="2:6">
-      <c r="B23" s="14"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="14"/>
+      <c r="B23" s="13"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1220,453 +1249,453 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
   <cols>
-    <col min="1" max="1" width="11.625" style="14" customWidth="1"/>
-    <col min="2" max="2" width="9" style="14"/>
-    <col min="3" max="3" width="10.25" style="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="7" width="9" style="14"/>
-    <col min="8" max="8" width="9.625" style="14" customWidth="1"/>
-    <col min="9" max="16384" width="9" style="14"/>
+    <col min="1" max="1" width="11.625" style="13" customWidth="1"/>
+    <col min="2" max="2" width="9" style="13"/>
+    <col min="3" max="3" width="10.25" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="9" style="13"/>
+    <col min="8" max="8" width="9.625" style="13" customWidth="1"/>
+    <col min="9" max="16384" width="9" style="13"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" ht="15" customHeight="1">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="F1" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="H1" s="20" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="16">
+      <c r="C2" s="15">
         <v>41981</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="E2" s="18">
+      <c r="E2" s="17">
         <v>9.9</v>
       </c>
-      <c r="F2" s="18">
+      <c r="F2" s="17">
         <v>1000</v>
       </c>
-      <c r="G2" s="18"/>
-      <c r="H2" s="25"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="24"/>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="18"/>
-      <c r="B3" s="18"/>
-      <c r="C3" s="26">
+      <c r="A3" s="17"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="25">
         <v>41985</v>
       </c>
-      <c r="D3" s="27" t="s">
+      <c r="D3" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="E3" s="30">
+      <c r="E3" s="29">
         <v>10.37</v>
       </c>
-      <c r="F3" s="30">
+      <c r="F3" s="29">
         <v>1000</v>
       </c>
-      <c r="G3" s="11">
+      <c r="G3" s="10">
         <v>4.5400000000000003E-2</v>
       </c>
-      <c r="H3" s="11">
+      <c r="H3" s="10">
         <f>G3/5</f>
         <v>9.0800000000000013E-3</v>
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="C4" s="16">
+      <c r="C4" s="15">
         <v>42003</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="18">
+      <c r="E4" s="17">
         <v>7.11</v>
       </c>
-      <c r="F4" s="18">
+      <c r="F4" s="17">
         <v>1600</v>
       </c>
-      <c r="G4" s="18"/>
-      <c r="H4" s="25"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="24"/>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="18"/>
-      <c r="B5" s="18"/>
-      <c r="C5" s="26">
+      <c r="A5" s="17"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="25">
         <v>42011</v>
       </c>
-      <c r="D5" s="27" t="s">
+      <c r="D5" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="30">
+      <c r="E5" s="29">
         <v>7.14</v>
       </c>
-      <c r="F5" s="30">
+      <c r="F5" s="29">
         <v>1600</v>
       </c>
-      <c r="G5" s="11">
+      <c r="G5" s="10">
         <v>2.2000000000000001E-3</v>
       </c>
-      <c r="H5" s="11">
+      <c r="H5" s="10">
         <f>G5/9</f>
         <v>2.4444444444444448E-4</v>
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="16">
+      <c r="C6" s="15">
         <v>41992</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="D6" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="E6" s="18">
+      <c r="E6" s="17">
         <v>12.52</v>
       </c>
-      <c r="F6" s="18">
+      <c r="F6" s="17">
         <v>800</v>
       </c>
-      <c r="G6" s="18"/>
-      <c r="H6" s="25"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="24"/>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="18"/>
-      <c r="B7" s="18"/>
-      <c r="C7" s="26">
+      <c r="A7" s="17"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="25">
         <v>42003</v>
       </c>
-      <c r="D7" s="27" t="s">
+      <c r="D7" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="E7" s="27">
+      <c r="E7" s="26">
         <v>13.9</v>
       </c>
-      <c r="F7" s="27">
+      <c r="F7" s="26">
         <v>800</v>
       </c>
-      <c r="G7" s="11">
+      <c r="G7" s="10">
         <v>0.108</v>
       </c>
-      <c r="H7" s="11">
+      <c r="H7" s="10">
         <f>G7/12</f>
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="16">
+      <c r="C8" s="15">
         <v>41985</v>
       </c>
-      <c r="D8" s="18" t="s">
+      <c r="D8" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="18">
+      <c r="E8" s="17">
         <v>3.47</v>
       </c>
-      <c r="F8" s="18">
+      <c r="F8" s="17">
         <v>3000</v>
       </c>
-      <c r="G8" s="18"/>
-      <c r="H8" s="25"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="24"/>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="18"/>
-      <c r="B9" s="18"/>
-      <c r="C9" s="28">
+      <c r="A9" s="17"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="27">
         <v>41992</v>
       </c>
-      <c r="D9" s="29" t="s">
+      <c r="D9" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="E9" s="29">
+      <c r="E9" s="28">
         <v>3.47</v>
       </c>
-      <c r="F9" s="29">
+      <c r="F9" s="28">
         <v>3000</v>
       </c>
-      <c r="G9" s="8">
+      <c r="G9" s="7">
         <v>-2E-3</v>
       </c>
-      <c r="H9" s="8">
+      <c r="H9" s="7">
         <f>G9/8</f>
         <v>-2.5000000000000001E-4</v>
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="18" t="s">
+      <c r="A10" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="B10" s="18" t="s">
+      <c r="B10" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="C10" s="16">
+      <c r="C10" s="15">
         <v>40695</v>
       </c>
-      <c r="D10" s="16" t="s">
+      <c r="D10" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="E10" s="18">
+      <c r="E10" s="17">
         <v>16.34</v>
       </c>
-      <c r="F10" s="18">
+      <c r="F10" s="17">
         <v>1080</v>
       </c>
-      <c r="G10" s="8"/>
-      <c r="H10" s="25"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="24"/>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="18"/>
-      <c r="B11" s="18"/>
-      <c r="C11" s="26">
+      <c r="A11" s="17"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="25">
         <v>41954</v>
       </c>
-      <c r="D11" s="27" t="s">
+      <c r="D11" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="E11" s="30">
+      <c r="E11" s="29">
         <v>27.55</v>
       </c>
-      <c r="F11" s="30">
+      <c r="F11" s="29">
         <v>780</v>
       </c>
-      <c r="G11" s="11"/>
-      <c r="H11" s="32"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="31"/>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="18"/>
-      <c r="B12" s="18"/>
-      <c r="C12" s="31">
+      <c r="A12" s="17"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="30">
         <v>41970</v>
       </c>
-      <c r="D12" s="30" t="s">
+      <c r="D12" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="E12" s="30">
+      <c r="E12" s="29">
         <v>30.2</v>
       </c>
-      <c r="F12" s="30">
+      <c r="F12" s="29">
         <v>300</v>
       </c>
-      <c r="G12" s="11">
+      <c r="G12" s="10">
         <v>0.72070000000000001</v>
       </c>
-      <c r="H12" s="32">
+      <c r="H12" s="31">
         <f>G12/1273</f>
         <v>5.6614296936370774E-4</v>
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="18" t="s">
+      <c r="A13" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="18" t="s">
+      <c r="B13" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="16">
+      <c r="C13" s="15">
         <v>42011</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D13" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="E13" s="18">
+      <c r="E13" s="17">
         <v>10.11</v>
       </c>
-      <c r="F13" s="18">
+      <c r="F13" s="17">
         <v>1100</v>
       </c>
-      <c r="G13" s="18"/>
-      <c r="H13" s="25"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="24"/>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="18"/>
-      <c r="B14" s="18"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
-      <c r="H14" s="25"/>
+      <c r="A14" s="17"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="24"/>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="18"/>
-      <c r="B15" s="18"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
-      <c r="H15" s="25"/>
+      <c r="A15" s="17"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="24"/>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="18"/>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
-      <c r="H16" s="25"/>
+      <c r="A16" s="17"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="24"/>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="18"/>
-      <c r="B17" s="18"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="25"/>
+      <c r="A17" s="17"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="24"/>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="18"/>
-      <c r="B18" s="18"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
-      <c r="H18" s="25"/>
+      <c r="A18" s="17"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="24"/>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="18"/>
-      <c r="B19" s="18"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="25"/>
+      <c r="A19" s="17"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="24"/>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="18"/>
-      <c r="B20" s="18"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
-      <c r="H20" s="25"/>
+      <c r="A20" s="17"/>
+      <c r="B20" s="17"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="17"/>
+      <c r="G20" s="17"/>
+      <c r="H20" s="24"/>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="18"/>
-      <c r="B21" s="18"/>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
-      <c r="H21" s="25"/>
+      <c r="A21" s="17"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="17"/>
+      <c r="H21" s="24"/>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="18"/>
-      <c r="B22" s="18"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="18"/>
-      <c r="H22" s="25"/>
+      <c r="A22" s="17"/>
+      <c r="B22" s="17"/>
+      <c r="C22" s="17"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="17"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="24"/>
     </row>
     <row r="23" spans="1:8">
-      <c r="A23" s="18"/>
-      <c r="B23" s="18"/>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
-      <c r="H23" s="25"/>
+      <c r="A23" s="17"/>
+      <c r="B23" s="17"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="24"/>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="18"/>
-      <c r="B24" s="18"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="18"/>
-      <c r="H24" s="25"/>
+      <c r="A24" s="17"/>
+      <c r="B24" s="17"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="17"/>
+      <c r="G24" s="17"/>
+      <c r="H24" s="24"/>
     </row>
     <row r="25" spans="1:8">
-      <c r="H25" s="24"/>
+      <c r="H25" s="23"/>
     </row>
     <row r="26" spans="1:8">
-      <c r="H26" s="24"/>
+      <c r="H26" s="23"/>
     </row>
     <row r="27" spans="1:8">
-      <c r="H27" s="24"/>
+      <c r="H27" s="23"/>
     </row>
     <row r="28" spans="1:8">
-      <c r="H28" s="24"/>
+      <c r="H28" s="23"/>
     </row>
     <row r="29" spans="1:8">
-      <c r="H29" s="24"/>
+      <c r="H29" s="23"/>
     </row>
     <row r="30" spans="1:8">
-      <c r="H30" s="24"/>
+      <c r="H30" s="23"/>
     </row>
     <row r="31" spans="1:8">
-      <c r="H31" s="24"/>
+      <c r="H31" s="23"/>
     </row>
     <row r="32" spans="1:8">
-      <c r="H32" s="24"/>
+      <c r="H32" s="23"/>
     </row>
     <row r="33" spans="8:8">
-      <c r="H33" s="24"/>
+      <c r="H33" s="23"/>
     </row>
     <row r="34" spans="8:8">
-      <c r="H34" s="24"/>
+      <c r="H34" s="23"/>
     </row>
     <row r="35" spans="8:8">
-      <c r="H35" s="24"/>
+      <c r="H35" s="23"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
new - transaction cause and each rate of return
</commit_message>
<xml_diff>
--- a/investment/record.xlsx
+++ b/investment/record.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="8220" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="8220" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="损益" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="54">
   <si>
     <t>日期</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -118,14 +118,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>收益率</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>日收益率</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>SZ-000671</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -178,6 +170,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>老婆</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>资金来源</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -187,6 +183,54 @@
   </si>
   <si>
     <t>我2014年终奖</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SZ-002155</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>辰州矿业</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SH-600773</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>西藏城投</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>我</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>日均收益率</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>交易收益率</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>单股收益率</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>交易原因</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>达到目标价 24，止盈</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>清仓锁定盈利</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>持股账号合并，从广发清空</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -265,7 +309,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -278,8 +322,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -302,13 +364,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -378,9 +477,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="10" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -399,10 +495,49 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="10" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="7" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="7" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="7" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="7" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="6" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
@@ -899,7 +1034,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
@@ -934,7 +1069,7 @@
         <v>1</v>
       </c>
       <c r="G1" s="20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -998,7 +1133,7 @@
         <v>191403.09</v>
       </c>
       <c r="G4" s="18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -1040,7 +1175,7 @@
         <v>198462.69999999998</v>
       </c>
       <c r="G6" s="18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -1247,10 +1382,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H35"/>
+  <dimension ref="A1:J48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
@@ -1258,12 +1393,15 @@
     <col min="1" max="1" width="11.625" style="13" customWidth="1"/>
     <col min="2" max="2" width="9" style="13"/>
     <col min="3" max="3" width="10.25" style="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="7" width="9" style="13"/>
+    <col min="4" max="6" width="9" style="13"/>
+    <col min="7" max="7" width="10.375" style="13" customWidth="1"/>
     <col min="8" max="8" width="9.625" style="13" customWidth="1"/>
-    <col min="9" max="16384" width="9" style="13"/>
+    <col min="9" max="9" width="12.375" style="13" customWidth="1"/>
+    <col min="10" max="10" width="30.125" style="13" customWidth="1"/>
+    <col min="11" max="16384" width="9" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:10" s="1" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="20" t="s">
         <v>16</v>
       </c>
@@ -1283,421 +1421,917 @@
         <v>20</v>
       </c>
       <c r="G1" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="H1" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="I1" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="J1" s="20" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" s="1" customFormat="1" ht="15" customHeight="1">
+      <c r="A2" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="35"/>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="15">
+        <v>41981</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="16">
+        <v>9.9</v>
+      </c>
+      <c r="F3" s="17">
+        <v>1000</v>
+      </c>
+      <c r="G3" s="17"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="17"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="24">
+        <v>41985</v>
+      </c>
+      <c r="D4" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="32">
+        <v>10.37</v>
+      </c>
+      <c r="F4" s="28">
+        <v>1000</v>
+      </c>
+      <c r="G4" s="10">
+        <v>4.5400000000000003E-2</v>
+      </c>
+      <c r="H4" s="10">
+        <f>G4/5</f>
+        <v>9.0800000000000013E-3</v>
+      </c>
+      <c r="I4" s="10">
+        <v>4.5400000000000003E-2</v>
+      </c>
+      <c r="J4" s="17"/>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="15">
+        <v>42003</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="16">
+        <v>7.11</v>
+      </c>
+      <c r="F5" s="17">
+        <v>1600</v>
+      </c>
+      <c r="G5" s="17"/>
+      <c r="H5" s="23"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="17"/>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="17"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="24">
+        <v>42011</v>
+      </c>
+      <c r="D6" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" s="32">
+        <v>7.14</v>
+      </c>
+      <c r="F6" s="28">
+        <v>1600</v>
+      </c>
+      <c r="G6" s="10">
+        <v>2.2000000000000001E-3</v>
+      </c>
+      <c r="H6" s="10">
+        <f>G6/9</f>
+        <v>2.4444444444444448E-4</v>
+      </c>
+      <c r="I6" s="10">
+        <v>2.2000000000000001E-3</v>
+      </c>
+      <c r="J6" s="17"/>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="H1" s="20" t="s">
+      <c r="B7" s="17" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" s="15">
-        <v>41981</v>
-      </c>
-      <c r="D2" s="17" t="s">
+      <c r="C7" s="15">
+        <v>41992</v>
+      </c>
+      <c r="D7" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="E2" s="17">
-        <v>9.9</v>
-      </c>
-      <c r="F2" s="17">
-        <v>1000</v>
-      </c>
-      <c r="G2" s="17"/>
-      <c r="H2" s="24"/>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="17"/>
-      <c r="B3" s="17"/>
-      <c r="C3" s="25">
+      <c r="E7" s="16">
+        <v>12.52</v>
+      </c>
+      <c r="F7" s="17">
+        <v>800</v>
+      </c>
+      <c r="G7" s="17"/>
+      <c r="H7" s="23"/>
+      <c r="I7" s="29"/>
+      <c r="J7" s="17"/>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="17"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="24">
+        <v>42003</v>
+      </c>
+      <c r="D8" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="33">
+        <v>13.9</v>
+      </c>
+      <c r="F8" s="25">
+        <v>800</v>
+      </c>
+      <c r="G8" s="10">
+        <v>0.108</v>
+      </c>
+      <c r="H8" s="10">
+        <f>G8/12</f>
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="I8" s="10">
+        <v>0.108</v>
+      </c>
+      <c r="J8" s="17"/>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="15">
         <v>41985</v>
       </c>
-      <c r="D3" s="26" t="s">
-        <v>35</v>
-      </c>
-      <c r="E3" s="29">
-        <v>10.37</v>
-      </c>
-      <c r="F3" s="29">
-        <v>1000</v>
-      </c>
-      <c r="G3" s="10">
-        <v>4.5400000000000003E-2</v>
-      </c>
-      <c r="H3" s="10">
-        <f>G3/5</f>
-        <v>9.0800000000000013E-3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="B4" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="C4" s="15">
-        <v>42003</v>
-      </c>
-      <c r="D4" s="17" t="s">
+      <c r="D9" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="17">
-        <v>7.11</v>
-      </c>
-      <c r="F4" s="17">
-        <v>1600</v>
-      </c>
-      <c r="G4" s="17"/>
-      <c r="H4" s="24"/>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="17"/>
-      <c r="B5" s="17"/>
-      <c r="C5" s="25">
+      <c r="E9" s="16">
+        <v>3.47</v>
+      </c>
+      <c r="F9" s="17">
+        <v>3000</v>
+      </c>
+      <c r="G9" s="17"/>
+      <c r="H9" s="23"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="17"/>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="17"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="26">
+        <v>41992</v>
+      </c>
+      <c r="D10" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" s="34">
+        <v>3.47</v>
+      </c>
+      <c r="F10" s="27">
+        <v>3000</v>
+      </c>
+      <c r="G10" s="7">
+        <v>-2E-3</v>
+      </c>
+      <c r="H10" s="7">
+        <f>G10/8</f>
+        <v>-2.5000000000000001E-4</v>
+      </c>
+      <c r="I10" s="7">
+        <v>-2E-3</v>
+      </c>
+      <c r="J10" s="17"/>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="15">
         <v>42011</v>
       </c>
-      <c r="D5" s="26" t="s">
-        <v>29</v>
-      </c>
-      <c r="E5" s="29">
-        <v>7.14</v>
-      </c>
-      <c r="F5" s="29">
-        <v>1600</v>
-      </c>
-      <c r="G5" s="10">
-        <v>2.2000000000000001E-3</v>
-      </c>
-      <c r="H5" s="10">
-        <f>G5/9</f>
-        <v>2.4444444444444448E-4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="B6" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="C6" s="15">
-        <v>41992</v>
-      </c>
-      <c r="D6" s="17" t="s">
+      <c r="D11" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="E6" s="17">
-        <v>12.52</v>
-      </c>
-      <c r="F6" s="17">
-        <v>800</v>
-      </c>
-      <c r="G6" s="17"/>
-      <c r="H6" s="24"/>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="17"/>
-      <c r="B7" s="17"/>
-      <c r="C7" s="25">
-        <v>42003</v>
-      </c>
-      <c r="D7" s="26" t="s">
-        <v>29</v>
-      </c>
-      <c r="E7" s="26">
-        <v>13.9</v>
-      </c>
-      <c r="F7" s="26">
-        <v>800</v>
-      </c>
-      <c r="G7" s="10">
-        <v>0.108</v>
-      </c>
-      <c r="H7" s="10">
-        <f>G7/12</f>
-        <v>8.9999999999999993E-3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="B8" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="C8" s="15">
-        <v>41985</v>
-      </c>
-      <c r="D8" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="E8" s="17">
-        <v>3.47</v>
-      </c>
-      <c r="F8" s="17">
-        <v>3000</v>
-      </c>
-      <c r="G8" s="17"/>
-      <c r="H8" s="24"/>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="17"/>
-      <c r="B9" s="17"/>
-      <c r="C9" s="27">
-        <v>41992</v>
-      </c>
-      <c r="D9" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="E9" s="28">
-        <v>3.47</v>
-      </c>
-      <c r="F9" s="28">
-        <v>3000</v>
-      </c>
-      <c r="G9" s="7">
-        <v>-2E-3</v>
-      </c>
-      <c r="H9" s="7">
-        <f>G9/8</f>
-        <v>-2.5000000000000001E-4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="B10" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="C10" s="15">
-        <v>40695</v>
-      </c>
-      <c r="D10" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="E10" s="17">
-        <v>16.34</v>
-      </c>
-      <c r="F10" s="17">
-        <v>1080</v>
-      </c>
-      <c r="G10" s="7"/>
-      <c r="H10" s="24"/>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11" s="17"/>
-      <c r="B11" s="17"/>
-      <c r="C11" s="25">
-        <v>41954</v>
-      </c>
-      <c r="D11" s="26" t="s">
-        <v>29</v>
-      </c>
-      <c r="E11" s="29">
-        <v>27.55</v>
-      </c>
-      <c r="F11" s="29">
-        <v>780</v>
-      </c>
-      <c r="G11" s="10"/>
-      <c r="H11" s="31"/>
-    </row>
-    <row r="12" spans="1:8">
+      <c r="E11" s="16">
+        <v>10.11</v>
+      </c>
+      <c r="F11" s="17">
+        <v>1100</v>
+      </c>
+      <c r="G11" s="17"/>
+      <c r="H11" s="23"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="17"/>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12" s="17"/>
       <c r="B12" s="17"/>
-      <c r="C12" s="30">
-        <v>41970</v>
-      </c>
-      <c r="D12" s="29" t="s">
-        <v>29</v>
-      </c>
-      <c r="E12" s="29">
-        <v>30.2</v>
-      </c>
-      <c r="F12" s="29">
-        <v>300</v>
-      </c>
-      <c r="G12" s="10">
-        <v>0.72070000000000001</v>
-      </c>
-      <c r="H12" s="31">
-        <f>G12/1273</f>
-        <v>5.6614296936370774E-4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="A13" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" s="15">
-        <v>42011</v>
-      </c>
-      <c r="D13" s="15" t="s">
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="23"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="17"/>
+    </row>
+    <row r="13" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A13" s="36" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" s="36"/>
+      <c r="C13" s="36"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="36"/>
+      <c r="G13" s="36"/>
+      <c r="H13" s="36"/>
+      <c r="I13" s="36"/>
+      <c r="J13" s="36"/>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="15">
+        <v>40695</v>
+      </c>
+      <c r="D14" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="E13" s="17">
-        <v>10.11</v>
-      </c>
-      <c r="F13" s="17">
-        <v>1100</v>
-      </c>
-      <c r="G13" s="17"/>
-      <c r="H13" s="24"/>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="A14" s="17"/>
-      <c r="B14" s="17"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="24"/>
-    </row>
-    <row r="15" spans="1:8">
+      <c r="E14" s="16">
+        <v>16.34</v>
+      </c>
+      <c r="F14" s="17">
+        <v>1080</v>
+      </c>
+      <c r="G14" s="7"/>
+      <c r="H14" s="23"/>
+      <c r="I14" s="17"/>
+      <c r="J14" s="17"/>
+    </row>
+    <row r="15" spans="1:10">
       <c r="A15" s="17"/>
       <c r="B15" s="17"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="17"/>
-      <c r="H15" s="24"/>
-    </row>
-    <row r="16" spans="1:8">
+      <c r="C15" s="15">
+        <v>41954</v>
+      </c>
+      <c r="D15" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="E15" s="4">
+        <v>27.55</v>
+      </c>
+      <c r="F15" s="6">
+        <v>780</v>
+      </c>
+      <c r="G15" s="10">
+        <v>0.68600000000000005</v>
+      </c>
+      <c r="H15" s="31">
+        <f>G15/1258</f>
+        <v>5.4531001589825127E-4</v>
+      </c>
+      <c r="I15" s="17"/>
+      <c r="J15" s="37" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
       <c r="A16" s="17"/>
       <c r="B16" s="17"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="24"/>
-    </row>
-    <row r="17" spans="1:8">
+      <c r="C16" s="30">
+        <v>41970</v>
+      </c>
+      <c r="D16" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="E16" s="32">
+        <v>30.2</v>
+      </c>
+      <c r="F16" s="28">
+        <v>300</v>
+      </c>
+      <c r="G16" s="10">
+        <v>0.84799999999999998</v>
+      </c>
+      <c r="H16" s="31">
+        <f>G16/1273</f>
+        <v>6.6614296936370779E-4</v>
+      </c>
+      <c r="I16" s="10">
+        <v>0.72070000000000001</v>
+      </c>
+      <c r="J16" s="37" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17" s="17"/>
       <c r="B17" s="17"/>
       <c r="C17" s="17"/>
       <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
+      <c r="E17" s="16"/>
       <c r="F17" s="17"/>
       <c r="G17" s="17"/>
-      <c r="H17" s="24"/>
-    </row>
-    <row r="18" spans="1:8">
-      <c r="A18" s="17"/>
-      <c r="B18" s="17"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="17"/>
+      <c r="H17" s="23"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="17"/>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" s="15">
+        <v>40524</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="E18" s="16">
+        <v>19.68</v>
+      </c>
+      <c r="F18" s="17">
+        <v>1820</v>
+      </c>
       <c r="G18" s="17"/>
-      <c r="H18" s="24"/>
-    </row>
-    <row r="19" spans="1:8">
+      <c r="H18" s="23"/>
+      <c r="I18" s="17"/>
+      <c r="J18" s="17"/>
+    </row>
+    <row r="19" spans="1:10">
       <c r="A19" s="17"/>
       <c r="B19" s="17"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="17"/>
+      <c r="C19" s="15">
+        <v>41858</v>
+      </c>
+      <c r="D19" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="E19" s="16">
+        <v>9.08</v>
+      </c>
+      <c r="F19" s="17">
+        <v>300</v>
+      </c>
       <c r="G19" s="17"/>
-      <c r="H19" s="24"/>
-    </row>
-    <row r="20" spans="1:8">
+      <c r="H19" s="23"/>
+      <c r="I19" s="17"/>
+      <c r="J19" s="17"/>
+    </row>
+    <row r="20" spans="1:10">
       <c r="A20" s="17"/>
       <c r="B20" s="17"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="17"/>
+      <c r="C20" s="15">
+        <v>41862</v>
+      </c>
+      <c r="D20" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="E20" s="16">
+        <v>9.18</v>
+      </c>
+      <c r="F20" s="17">
+        <v>200</v>
+      </c>
       <c r="G20" s="17"/>
-      <c r="H20" s="24"/>
-    </row>
-    <row r="21" spans="1:8">
+      <c r="H20" s="23"/>
+      <c r="I20" s="17"/>
+      <c r="J20" s="17"/>
+    </row>
+    <row r="21" spans="1:10">
       <c r="A21" s="17"/>
       <c r="B21" s="17"/>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="17"/>
+      <c r="C21" s="15">
+        <v>41893</v>
+      </c>
+      <c r="D21" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="E21" s="16">
+        <v>8.6</v>
+      </c>
+      <c r="F21" s="17">
+        <v>300</v>
+      </c>
       <c r="G21" s="17"/>
-      <c r="H21" s="24"/>
-    </row>
-    <row r="22" spans="1:8">
+      <c r="H21" s="23"/>
+      <c r="I21" s="17"/>
+      <c r="J21" s="17"/>
+    </row>
+    <row r="22" spans="1:10">
       <c r="A22" s="17"/>
       <c r="B22" s="17"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="17"/>
-      <c r="E22" s="17"/>
-      <c r="F22" s="17"/>
+      <c r="C22" s="15">
+        <v>41976</v>
+      </c>
+      <c r="D22" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="E22" s="16">
+        <v>10.63</v>
+      </c>
+      <c r="F22" s="17">
+        <v>2200</v>
+      </c>
       <c r="G22" s="17"/>
-      <c r="H22" s="24"/>
-    </row>
-    <row r="23" spans="1:8">
+      <c r="H22" s="23"/>
+      <c r="I22" s="17"/>
+      <c r="J22" s="17"/>
+    </row>
+    <row r="23" spans="1:10">
       <c r="A23" s="17"/>
       <c r="B23" s="17"/>
-      <c r="C23" s="17"/>
-      <c r="D23" s="17"/>
-      <c r="E23" s="17"/>
-      <c r="F23" s="17"/>
+      <c r="C23" s="15">
+        <v>41988</v>
+      </c>
+      <c r="D23" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="E23" s="16">
+        <v>9.98</v>
+      </c>
+      <c r="F23" s="17">
+        <v>200</v>
+      </c>
       <c r="G23" s="17"/>
-      <c r="H23" s="24"/>
-    </row>
-    <row r="24" spans="1:8">
+      <c r="H23" s="23"/>
+      <c r="I23" s="17"/>
+      <c r="J23" s="17"/>
+    </row>
+    <row r="24" spans="1:10">
       <c r="A24" s="17"/>
       <c r="B24" s="17"/>
-      <c r="C24" s="17"/>
-      <c r="D24" s="17"/>
-      <c r="E24" s="17"/>
-      <c r="F24" s="17"/>
+      <c r="C24" s="15">
+        <v>41988</v>
+      </c>
+      <c r="D24" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="E24" s="16">
+        <v>9.9700000000000006</v>
+      </c>
+      <c r="F24" s="17">
+        <v>600</v>
+      </c>
       <c r="G24" s="17"/>
-      <c r="H24" s="24"/>
-    </row>
-    <row r="25" spans="1:8">
-      <c r="H25" s="23"/>
-    </row>
-    <row r="26" spans="1:8">
-      <c r="H26" s="23"/>
-    </row>
-    <row r="27" spans="1:8">
-      <c r="H27" s="23"/>
-    </row>
-    <row r="28" spans="1:8">
-      <c r="H28" s="23"/>
-    </row>
-    <row r="29" spans="1:8">
+      <c r="H24" s="23"/>
+      <c r="I24" s="17"/>
+      <c r="J24" s="17"/>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" s="17"/>
+      <c r="B25" s="17"/>
+      <c r="C25" s="15">
+        <v>41995</v>
+      </c>
+      <c r="D25" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="E25" s="16">
+        <v>10.4</v>
+      </c>
+      <c r="F25" s="17">
+        <v>1820</v>
+      </c>
+      <c r="G25" s="41">
+        <v>-0.47149999999999997</v>
+      </c>
+      <c r="H25" s="42">
+        <f>G25/1463</f>
+        <v>-3.22282980177717E-4</v>
+      </c>
+      <c r="I25" s="17"/>
+      <c r="J25" s="38" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26" s="17"/>
+      <c r="B26" s="17"/>
+      <c r="C26" s="15">
+        <v>41995</v>
+      </c>
+      <c r="D26" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="E26" s="16">
+        <v>10.4</v>
+      </c>
+      <c r="F26" s="17">
+        <v>300</v>
+      </c>
+      <c r="G26" s="43">
+        <f>(E26-E19)/E19</f>
+        <v>0.14537444933920707</v>
+      </c>
+      <c r="H26" s="31">
+        <f>G26/138</f>
+        <v>1.0534380386899064E-3</v>
+      </c>
+      <c r="I26" s="17"/>
+      <c r="J26" s="39"/>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27" s="17"/>
+      <c r="B27" s="17"/>
+      <c r="C27" s="15">
+        <v>41995</v>
+      </c>
+      <c r="D27" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="E27" s="16">
+        <v>10.4</v>
+      </c>
+      <c r="F27" s="17">
+        <v>200</v>
+      </c>
+      <c r="G27" s="43">
+        <f>(E27-E20)/E20</f>
+        <v>0.13289760348583884</v>
+      </c>
+      <c r="H27" s="31">
+        <f>G27/134</f>
+        <v>9.9177316034208102E-4</v>
+      </c>
+      <c r="I27" s="17"/>
+      <c r="J27" s="39"/>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28" s="17"/>
+      <c r="B28" s="17"/>
+      <c r="C28" s="15">
+        <v>41995</v>
+      </c>
+      <c r="D28" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="E28" s="16">
+        <v>10.4</v>
+      </c>
+      <c r="F28" s="17">
+        <v>300</v>
+      </c>
+      <c r="G28" s="43">
+        <f>(E28-E21)/E21</f>
+        <v>0.20930232558139544</v>
+      </c>
+      <c r="H28" s="31">
+        <f>G28/103</f>
+        <v>2.0320614134116061E-3</v>
+      </c>
+      <c r="I28" s="17"/>
+      <c r="J28" s="40"/>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="A29" s="17"/>
+      <c r="B29" s="17"/>
+      <c r="C29" s="15">
+        <v>42039</v>
+      </c>
+      <c r="D29" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="E29" s="16">
+        <v>10.75</v>
+      </c>
+      <c r="F29" s="17">
+        <v>2000</v>
+      </c>
+      <c r="G29" s="41"/>
       <c r="H29" s="23"/>
-    </row>
-    <row r="30" spans="1:8">
+      <c r="I29" s="17"/>
+      <c r="J29" s="17"/>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="A30" s="17"/>
+      <c r="B30" s="17"/>
+      <c r="C30" s="15">
+        <v>42051</v>
+      </c>
+      <c r="D30" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="E30" s="16">
+        <v>10.51</v>
+      </c>
+      <c r="F30" s="17">
+        <v>2000</v>
+      </c>
+      <c r="G30" s="41"/>
       <c r="H30" s="23"/>
-    </row>
-    <row r="31" spans="1:8">
+      <c r="I30" s="17"/>
+      <c r="J30" s="17"/>
+    </row>
+    <row r="31" spans="1:10">
+      <c r="A31" s="17"/>
+      <c r="B31" s="17"/>
+      <c r="C31" s="17"/>
+      <c r="D31" s="17"/>
+      <c r="E31" s="16"/>
+      <c r="F31" s="17"/>
+      <c r="G31" s="17"/>
       <c r="H31" s="23"/>
-    </row>
-    <row r="32" spans="1:8">
+      <c r="I31" s="17"/>
+      <c r="J31" s="17"/>
+    </row>
+    <row r="32" spans="1:10">
+      <c r="A32" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="B32" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="C32" s="15">
+        <v>41971</v>
+      </c>
+      <c r="D32" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="E32" s="16">
+        <v>12.47</v>
+      </c>
+      <c r="F32" s="17">
+        <v>2000</v>
+      </c>
+      <c r="G32" s="17"/>
       <c r="H32" s="23"/>
-    </row>
-    <row r="33" spans="8:8">
+      <c r="I32" s="17"/>
+      <c r="J32" s="17"/>
+    </row>
+    <row r="33" spans="1:10">
+      <c r="A33" s="17"/>
+      <c r="B33" s="17"/>
+      <c r="C33" s="15">
+        <v>41995</v>
+      </c>
+      <c r="D33" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="E33" s="16">
+        <v>12.99</v>
+      </c>
+      <c r="F33" s="17">
+        <v>1200</v>
+      </c>
+      <c r="G33" s="17"/>
       <c r="H33" s="23"/>
-    </row>
-    <row r="34" spans="8:8">
+      <c r="I33" s="17"/>
+      <c r="J33" s="17"/>
+    </row>
+    <row r="34" spans="1:10">
+      <c r="A34" s="17"/>
+      <c r="B34" s="17"/>
+      <c r="C34" s="15">
+        <v>41997</v>
+      </c>
+      <c r="D34" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="E34" s="16">
+        <v>12.02</v>
+      </c>
+      <c r="F34" s="17">
+        <v>1800</v>
+      </c>
+      <c r="G34" s="17"/>
       <c r="H34" s="23"/>
-    </row>
-    <row r="35" spans="8:8">
+      <c r="I34" s="17"/>
+      <c r="J34" s="17"/>
+    </row>
+    <row r="35" spans="1:10">
+      <c r="A35" s="17"/>
+      <c r="B35" s="17"/>
+      <c r="C35" s="17"/>
+      <c r="D35" s="17"/>
+      <c r="E35" s="17"/>
+      <c r="F35" s="17"/>
+      <c r="G35" s="17"/>
       <c r="H35" s="23"/>
+      <c r="I35" s="17"/>
+      <c r="J35" s="17"/>
+    </row>
+    <row r="36" spans="1:10">
+      <c r="A36" s="17"/>
+      <c r="B36" s="17"/>
+      <c r="C36" s="17"/>
+      <c r="D36" s="17"/>
+      <c r="E36" s="17"/>
+      <c r="F36" s="17"/>
+      <c r="G36" s="17"/>
+      <c r="H36" s="23"/>
+      <c r="I36" s="17"/>
+      <c r="J36" s="17"/>
+    </row>
+    <row r="37" spans="1:10">
+      <c r="A37" s="17"/>
+      <c r="B37" s="17"/>
+      <c r="C37" s="17"/>
+      <c r="D37" s="17"/>
+      <c r="E37" s="17"/>
+      <c r="F37" s="17"/>
+      <c r="G37" s="17"/>
+      <c r="H37" s="23"/>
+      <c r="I37" s="17"/>
+      <c r="J37" s="17"/>
+    </row>
+    <row r="38" spans="1:10">
+      <c r="A38" s="17"/>
+      <c r="B38" s="17"/>
+      <c r="C38" s="17"/>
+      <c r="D38" s="17"/>
+      <c r="E38" s="17"/>
+      <c r="F38" s="17"/>
+      <c r="G38" s="17"/>
+      <c r="H38" s="23"/>
+      <c r="I38" s="17"/>
+      <c r="J38" s="17"/>
+    </row>
+    <row r="39" spans="1:10">
+      <c r="A39" s="17"/>
+      <c r="B39" s="17"/>
+      <c r="C39" s="17"/>
+      <c r="D39" s="17"/>
+      <c r="E39" s="17"/>
+      <c r="F39" s="17"/>
+      <c r="G39" s="17"/>
+      <c r="H39" s="23"/>
+      <c r="I39" s="17"/>
+      <c r="J39" s="17"/>
+    </row>
+    <row r="40" spans="1:10">
+      <c r="A40" s="17"/>
+      <c r="B40" s="17"/>
+      <c r="C40" s="17"/>
+      <c r="D40" s="17"/>
+      <c r="E40" s="17"/>
+      <c r="F40" s="17"/>
+      <c r="G40" s="17"/>
+      <c r="H40" s="23"/>
+      <c r="I40" s="17"/>
+      <c r="J40" s="17"/>
+    </row>
+    <row r="41" spans="1:10">
+      <c r="A41" s="17"/>
+      <c r="B41" s="17"/>
+      <c r="C41" s="17"/>
+      <c r="D41" s="17"/>
+      <c r="E41" s="17"/>
+      <c r="F41" s="17"/>
+      <c r="G41" s="17"/>
+      <c r="H41" s="23"/>
+      <c r="I41" s="17"/>
+      <c r="J41" s="17"/>
+    </row>
+    <row r="42" spans="1:10">
+      <c r="A42" s="17"/>
+      <c r="B42" s="17"/>
+      <c r="C42" s="17"/>
+      <c r="D42" s="17"/>
+      <c r="E42" s="17"/>
+      <c r="F42" s="17"/>
+      <c r="G42" s="17"/>
+      <c r="H42" s="17"/>
+      <c r="I42" s="17"/>
+      <c r="J42" s="17"/>
+    </row>
+    <row r="43" spans="1:10">
+      <c r="A43" s="17"/>
+      <c r="B43" s="17"/>
+      <c r="C43" s="17"/>
+      <c r="D43" s="17"/>
+      <c r="E43" s="17"/>
+      <c r="F43" s="17"/>
+      <c r="G43" s="17"/>
+      <c r="H43" s="17"/>
+      <c r="I43" s="17"/>
+      <c r="J43" s="17"/>
+    </row>
+    <row r="44" spans="1:10">
+      <c r="A44" s="17"/>
+      <c r="B44" s="17"/>
+      <c r="C44" s="17"/>
+      <c r="D44" s="17"/>
+      <c r="E44" s="17"/>
+      <c r="F44" s="17"/>
+      <c r="G44" s="17"/>
+      <c r="H44" s="17"/>
+      <c r="I44" s="17"/>
+      <c r="J44" s="17"/>
+    </row>
+    <row r="45" spans="1:10">
+      <c r="A45" s="17"/>
+      <c r="B45" s="17"/>
+      <c r="C45" s="17"/>
+      <c r="D45" s="17"/>
+      <c r="E45" s="17"/>
+      <c r="F45" s="17"/>
+      <c r="G45" s="17"/>
+      <c r="H45" s="17"/>
+      <c r="I45" s="17"/>
+      <c r="J45" s="17"/>
+    </row>
+    <row r="46" spans="1:10">
+      <c r="A46" s="17"/>
+      <c r="B46" s="17"/>
+      <c r="C46" s="17"/>
+      <c r="D46" s="17"/>
+      <c r="E46" s="17"/>
+      <c r="F46" s="17"/>
+      <c r="G46" s="17"/>
+      <c r="H46" s="17"/>
+      <c r="I46" s="17"/>
+      <c r="J46" s="17"/>
+    </row>
+    <row r="47" spans="1:10">
+      <c r="A47" s="17"/>
+      <c r="B47" s="17"/>
+      <c r="C47" s="17"/>
+      <c r="D47" s="17"/>
+      <c r="E47" s="17"/>
+      <c r="F47" s="17"/>
+      <c r="G47" s="17"/>
+      <c r="H47" s="17"/>
+      <c r="I47" s="17"/>
+      <c r="J47" s="17"/>
+    </row>
+    <row r="48" spans="1:10">
+      <c r="A48" s="17"/>
+      <c r="B48" s="17"/>
+      <c r="C48" s="17"/>
+      <c r="D48" s="17"/>
+      <c r="E48" s="17"/>
+      <c r="F48" s="17"/>
+      <c r="G48" s="17"/>
+      <c r="H48" s="17"/>
+      <c r="I48" s="17"/>
+      <c r="J48" s="17"/>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="J25:J28"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A13:J13"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
new - transaction cause
</commit_message>
<xml_diff>
--- a/investment/record.xlsx
+++ b/investment/record.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="58">
   <si>
     <t>日期</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -231,6 +231,22 @@
   </si>
   <si>
     <t>持股账号合并，从广发清空</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>股票转移回补，因中间停牌一周，买回晚了</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>加仓潜伏资源板块，等待周期反转到来</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>主题投资买入</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>加仓买入补足仓位，国企改革、锂电、西藏等概念题材</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -407,7 +423,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -519,6 +535,9 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -539,6 +558,9 @@
     </xf>
     <xf numFmtId="10" fontId="6" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1384,8 +1406,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="M33" sqref="M33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
@@ -1397,7 +1419,7 @@
     <col min="7" max="7" width="10.375" style="13" customWidth="1"/>
     <col min="8" max="8" width="9.625" style="13" customWidth="1"/>
     <col min="9" max="9" width="12.375" style="13" customWidth="1"/>
-    <col min="10" max="10" width="30.125" style="13" customWidth="1"/>
+    <col min="10" max="10" width="36" style="37" customWidth="1"/>
     <col min="11" max="16384" width="9" style="13"/>
   </cols>
   <sheetData>
@@ -1469,7 +1491,7 @@
       <c r="G3" s="17"/>
       <c r="H3" s="23"/>
       <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
+      <c r="J3" s="38"/>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="17"/>
@@ -1496,7 +1518,7 @@
       <c r="I4" s="10">
         <v>4.5400000000000003E-2</v>
       </c>
-      <c r="J4" s="17"/>
+      <c r="J4" s="38"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="17" t="s">
@@ -1520,7 +1542,7 @@
       <c r="G5" s="17"/>
       <c r="H5" s="23"/>
       <c r="I5" s="17"/>
-      <c r="J5" s="17"/>
+      <c r="J5" s="38"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="17"/>
@@ -1547,7 +1569,7 @@
       <c r="I6" s="10">
         <v>2.2000000000000001E-3</v>
       </c>
-      <c r="J6" s="17"/>
+      <c r="J6" s="38"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="17" t="s">
@@ -1571,7 +1593,7 @@
       <c r="G7" s="17"/>
       <c r="H7" s="23"/>
       <c r="I7" s="29"/>
-      <c r="J7" s="17"/>
+      <c r="J7" s="38"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="17"/>
@@ -1598,7 +1620,7 @@
       <c r="I8" s="10">
         <v>0.108</v>
       </c>
-      <c r="J8" s="17"/>
+      <c r="J8" s="38"/>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" s="17" t="s">
@@ -1622,7 +1644,7 @@
       <c r="G9" s="17"/>
       <c r="H9" s="23"/>
       <c r="I9" s="17"/>
-      <c r="J9" s="17"/>
+      <c r="J9" s="38"/>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" s="17"/>
@@ -1649,7 +1671,7 @@
       <c r="I10" s="7">
         <v>-2E-3</v>
       </c>
-      <c r="J10" s="17"/>
+      <c r="J10" s="38"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="17" t="s">
@@ -1673,7 +1695,7 @@
       <c r="G11" s="17"/>
       <c r="H11" s="23"/>
       <c r="I11" s="17"/>
-      <c r="J11" s="17"/>
+      <c r="J11" s="38"/>
     </row>
     <row r="12" spans="1:10">
       <c r="A12" s="17"/>
@@ -1685,7 +1707,7 @@
       <c r="G12" s="17"/>
       <c r="H12" s="23"/>
       <c r="I12" s="17"/>
-      <c r="J12" s="17"/>
+      <c r="J12" s="38"/>
     </row>
     <row r="13" spans="1:10" ht="15.75" customHeight="1">
       <c r="A13" s="36" t="s">
@@ -1723,7 +1745,7 @@
       <c r="G14" s="7"/>
       <c r="H14" s="23"/>
       <c r="I14" s="17"/>
-      <c r="J14" s="17"/>
+      <c r="J14" s="38"/>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" s="17"/>
@@ -1748,7 +1770,7 @@
         <v>5.4531001589825127E-4</v>
       </c>
       <c r="I15" s="17"/>
-      <c r="J15" s="37" t="s">
+      <c r="J15" s="38" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1777,7 +1799,7 @@
       <c r="I16" s="10">
         <v>0.72070000000000001</v>
       </c>
-      <c r="J16" s="37" t="s">
+      <c r="J16" s="38" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1791,7 +1813,7 @@
       <c r="G17" s="17"/>
       <c r="H17" s="23"/>
       <c r="I17" s="17"/>
-      <c r="J17" s="17"/>
+      <c r="J17" s="38"/>
     </row>
     <row r="18" spans="1:10">
       <c r="A18" s="17" t="s">
@@ -1815,7 +1837,7 @@
       <c r="G18" s="17"/>
       <c r="H18" s="23"/>
       <c r="I18" s="17"/>
-      <c r="J18" s="17"/>
+      <c r="J18" s="38"/>
     </row>
     <row r="19" spans="1:10">
       <c r="A19" s="17"/>
@@ -1835,7 +1857,7 @@
       <c r="G19" s="17"/>
       <c r="H19" s="23"/>
       <c r="I19" s="17"/>
-      <c r="J19" s="17"/>
+      <c r="J19" s="38"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="17"/>
@@ -1855,7 +1877,7 @@
       <c r="G20" s="17"/>
       <c r="H20" s="23"/>
       <c r="I20" s="17"/>
-      <c r="J20" s="17"/>
+      <c r="J20" s="38"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="17"/>
@@ -1875,7 +1897,7 @@
       <c r="G21" s="17"/>
       <c r="H21" s="23"/>
       <c r="I21" s="17"/>
-      <c r="J21" s="17"/>
+      <c r="J21" s="38"/>
     </row>
     <row r="22" spans="1:10">
       <c r="A22" s="17"/>
@@ -1895,7 +1917,7 @@
       <c r="G22" s="17"/>
       <c r="H22" s="23"/>
       <c r="I22" s="17"/>
-      <c r="J22" s="17"/>
+      <c r="J22" s="38"/>
     </row>
     <row r="23" spans="1:10">
       <c r="A23" s="17"/>
@@ -1915,7 +1937,7 @@
       <c r="G23" s="17"/>
       <c r="H23" s="23"/>
       <c r="I23" s="17"/>
-      <c r="J23" s="17"/>
+      <c r="J23" s="38"/>
     </row>
     <row r="24" spans="1:10">
       <c r="A24" s="17"/>
@@ -1935,7 +1957,7 @@
       <c r="G24" s="17"/>
       <c r="H24" s="23"/>
       <c r="I24" s="17"/>
-      <c r="J24" s="17"/>
+      <c r="J24" s="38"/>
     </row>
     <row r="25" spans="1:10">
       <c r="A25" s="17"/>
@@ -1952,15 +1974,15 @@
       <c r="F25" s="17">
         <v>1820</v>
       </c>
-      <c r="G25" s="41">
+      <c r="G25" s="42">
         <v>-0.47149999999999997</v>
       </c>
-      <c r="H25" s="42">
+      <c r="H25" s="43">
         <f>G25/1463</f>
         <v>-3.22282980177717E-4</v>
       </c>
       <c r="I25" s="17"/>
-      <c r="J25" s="38" t="s">
+      <c r="J25" s="39" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1979,7 +2001,7 @@
       <c r="F26" s="17">
         <v>300</v>
       </c>
-      <c r="G26" s="43">
+      <c r="G26" s="44">
         <f>(E26-E19)/E19</f>
         <v>0.14537444933920707</v>
       </c>
@@ -1988,7 +2010,7 @@
         <v>1.0534380386899064E-3</v>
       </c>
       <c r="I26" s="17"/>
-      <c r="J26" s="39"/>
+      <c r="J26" s="40"/>
     </row>
     <row r="27" spans="1:10">
       <c r="A27" s="17"/>
@@ -2005,7 +2027,7 @@
       <c r="F27" s="17">
         <v>200</v>
       </c>
-      <c r="G27" s="43">
+      <c r="G27" s="44">
         <f>(E27-E20)/E20</f>
         <v>0.13289760348583884</v>
       </c>
@@ -2014,7 +2036,7 @@
         <v>9.9177316034208102E-4</v>
       </c>
       <c r="I27" s="17"/>
-      <c r="J27" s="39"/>
+      <c r="J27" s="40"/>
     </row>
     <row r="28" spans="1:10">
       <c r="A28" s="17"/>
@@ -2031,7 +2053,7 @@
       <c r="F28" s="17">
         <v>300</v>
       </c>
-      <c r="G28" s="43">
+      <c r="G28" s="44">
         <f>(E28-E21)/E21</f>
         <v>0.20930232558139544</v>
       </c>
@@ -2040,7 +2062,7 @@
         <v>2.0320614134116061E-3</v>
       </c>
       <c r="I28" s="17"/>
-      <c r="J28" s="40"/>
+      <c r="J28" s="41"/>
     </row>
     <row r="29" spans="1:10">
       <c r="A29" s="17"/>
@@ -2057,10 +2079,12 @@
       <c r="F29" s="17">
         <v>2000</v>
       </c>
-      <c r="G29" s="41"/>
+      <c r="G29" s="42"/>
       <c r="H29" s="23"/>
       <c r="I29" s="17"/>
-      <c r="J29" s="17"/>
+      <c r="J29" s="38" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="30" spans="1:10">
       <c r="A30" s="17"/>
@@ -2077,10 +2101,12 @@
       <c r="F30" s="17">
         <v>2000</v>
       </c>
-      <c r="G30" s="41"/>
+      <c r="G30" s="42"/>
       <c r="H30" s="23"/>
       <c r="I30" s="17"/>
-      <c r="J30" s="17"/>
+      <c r="J30" s="38" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="31" spans="1:10">
       <c r="A31" s="17"/>
@@ -2092,7 +2118,7 @@
       <c r="G31" s="17"/>
       <c r="H31" s="23"/>
       <c r="I31" s="17"/>
-      <c r="J31" s="17"/>
+      <c r="J31" s="38"/>
     </row>
     <row r="32" spans="1:10">
       <c r="A32" s="17" t="s">
@@ -2116,7 +2142,9 @@
       <c r="G32" s="17"/>
       <c r="H32" s="23"/>
       <c r="I32" s="17"/>
-      <c r="J32" s="17"/>
+      <c r="J32" s="38" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="33" spans="1:10">
       <c r="A33" s="17"/>
@@ -2136,7 +2164,9 @@
       <c r="G33" s="17"/>
       <c r="H33" s="23"/>
       <c r="I33" s="17"/>
-      <c r="J33" s="17"/>
+      <c r="J33" s="45" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="34" spans="1:10">
       <c r="A34" s="17"/>
@@ -2156,7 +2186,7 @@
       <c r="G34" s="17"/>
       <c r="H34" s="23"/>
       <c r="I34" s="17"/>
-      <c r="J34" s="17"/>
+      <c r="J34" s="41"/>
     </row>
     <row r="35" spans="1:10">
       <c r="A35" s="17"/>
@@ -2168,7 +2198,7 @@
       <c r="G35" s="17"/>
       <c r="H35" s="23"/>
       <c r="I35" s="17"/>
-      <c r="J35" s="17"/>
+      <c r="J35" s="38"/>
     </row>
     <row r="36" spans="1:10">
       <c r="A36" s="17"/>
@@ -2180,7 +2210,7 @@
       <c r="G36" s="17"/>
       <c r="H36" s="23"/>
       <c r="I36" s="17"/>
-      <c r="J36" s="17"/>
+      <c r="J36" s="38"/>
     </row>
     <row r="37" spans="1:10">
       <c r="A37" s="17"/>
@@ -2192,7 +2222,7 @@
       <c r="G37" s="17"/>
       <c r="H37" s="23"/>
       <c r="I37" s="17"/>
-      <c r="J37" s="17"/>
+      <c r="J37" s="38"/>
     </row>
     <row r="38" spans="1:10">
       <c r="A38" s="17"/>
@@ -2204,7 +2234,7 @@
       <c r="G38" s="17"/>
       <c r="H38" s="23"/>
       <c r="I38" s="17"/>
-      <c r="J38" s="17"/>
+      <c r="J38" s="38"/>
     </row>
     <row r="39" spans="1:10">
       <c r="A39" s="17"/>
@@ -2216,7 +2246,7 @@
       <c r="G39" s="17"/>
       <c r="H39" s="23"/>
       <c r="I39" s="17"/>
-      <c r="J39" s="17"/>
+      <c r="J39" s="38"/>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="17"/>
@@ -2228,7 +2258,7 @@
       <c r="G40" s="17"/>
       <c r="H40" s="23"/>
       <c r="I40" s="17"/>
-      <c r="J40" s="17"/>
+      <c r="J40" s="38"/>
     </row>
     <row r="41" spans="1:10">
       <c r="A41" s="17"/>
@@ -2240,7 +2270,7 @@
       <c r="G41" s="17"/>
       <c r="H41" s="23"/>
       <c r="I41" s="17"/>
-      <c r="J41" s="17"/>
+      <c r="J41" s="38"/>
     </row>
     <row r="42" spans="1:10">
       <c r="A42" s="17"/>
@@ -2252,7 +2282,7 @@
       <c r="G42" s="17"/>
       <c r="H42" s="17"/>
       <c r="I42" s="17"/>
-      <c r="J42" s="17"/>
+      <c r="J42" s="38"/>
     </row>
     <row r="43" spans="1:10">
       <c r="A43" s="17"/>
@@ -2264,7 +2294,7 @@
       <c r="G43" s="17"/>
       <c r="H43" s="17"/>
       <c r="I43" s="17"/>
-      <c r="J43" s="17"/>
+      <c r="J43" s="38"/>
     </row>
     <row r="44" spans="1:10">
       <c r="A44" s="17"/>
@@ -2276,7 +2306,7 @@
       <c r="G44" s="17"/>
       <c r="H44" s="17"/>
       <c r="I44" s="17"/>
-      <c r="J44" s="17"/>
+      <c r="J44" s="38"/>
     </row>
     <row r="45" spans="1:10">
       <c r="A45" s="17"/>
@@ -2288,7 +2318,7 @@
       <c r="G45" s="17"/>
       <c r="H45" s="17"/>
       <c r="I45" s="17"/>
-      <c r="J45" s="17"/>
+      <c r="J45" s="38"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="17"/>
@@ -2300,7 +2330,7 @@
       <c r="G46" s="17"/>
       <c r="H46" s="17"/>
       <c r="I46" s="17"/>
-      <c r="J46" s="17"/>
+      <c r="J46" s="38"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="17"/>
@@ -2312,7 +2342,7 @@
       <c r="G47" s="17"/>
       <c r="H47" s="17"/>
       <c r="I47" s="17"/>
-      <c r="J47" s="17"/>
+      <c r="J47" s="38"/>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="17"/>
@@ -2324,11 +2354,12 @@
       <c r="G48" s="17"/>
       <c r="H48" s="17"/>
       <c r="I48" s="17"/>
-      <c r="J48" s="17"/>
+      <c r="J48" s="38"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="J25:J28"/>
+    <mergeCell ref="J33:J34"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A13:J13"/>
   </mergeCells>

</xml_diff>